<commit_message>
edit in improvements from PC
</commit_message>
<xml_diff>
--- a/r2fu.wide.data.xlsx
+++ b/r2fu.wide.data.xlsx
@@ -730,7 +730,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C3">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C6">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C7">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C8">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C9">
@@ -1615,7 +1615,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C11">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C12">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C13">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C14">
@@ -2143,7 +2143,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C16">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C17">
@@ -2491,7 +2491,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C19">
@@ -2620,7 +2620,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C20">
@@ -3007,7 +3007,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C23">
@@ -3175,7 +3175,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C24">
@@ -3484,7 +3484,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C27">
@@ -3535,7 +3535,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C28">
@@ -3625,7 +3625,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C29">
@@ -3922,7 +3922,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C31">
@@ -4090,7 +4090,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C32">
@@ -4258,7 +4258,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C33">
@@ -4426,7 +4426,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C34">
@@ -4594,7 +4594,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C35">
@@ -4645,7 +4645,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C36">
@@ -4864,7 +4864,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C38">
@@ -5047,7 +5047,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C40">
@@ -5098,7 +5098,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C41">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C42">
@@ -5290,7 +5290,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C43">
@@ -5419,7 +5419,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C44">
@@ -5845,7 +5845,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C47">
@@ -6130,7 +6130,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C51">
@@ -6181,7 +6181,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C52">
@@ -6349,7 +6349,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C53">
@@ -6517,7 +6517,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C54">
@@ -6697,7 +6697,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C56">
@@ -6814,7 +6814,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C57">
@@ -6946,7 +6946,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C58">
@@ -7114,7 +7114,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C59">
@@ -7165,7 +7165,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C60">
@@ -7294,7 +7294,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C61">
@@ -7384,7 +7384,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C62">
@@ -7564,7 +7564,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C64">
@@ -7615,7 +7615,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C65">
@@ -7783,7 +7783,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C66">
@@ -7963,7 +7963,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C68">
@@ -8182,7 +8182,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C70">
@@ -8440,7 +8440,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C72">
@@ -8608,7 +8608,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C73">
@@ -8995,7 +8995,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C76">
@@ -9046,7 +9046,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C77">
@@ -9214,7 +9214,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C78">
@@ -9382,7 +9382,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C79">
@@ -9679,7 +9679,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C81">
@@ -9937,7 +9937,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C83">
@@ -10066,7 +10066,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C84">
@@ -10234,7 +10234,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C85">
@@ -10324,7 +10324,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C86">
@@ -10453,7 +10453,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C87">
@@ -10504,7 +10504,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C88">
@@ -10762,7 +10762,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C90">
@@ -10852,7 +10852,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C91">
@@ -11149,7 +11149,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C93">
@@ -11458,7 +11458,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C96">
@@ -11626,7 +11626,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C97">
@@ -11845,7 +11845,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C99">
@@ -11974,7 +11974,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C100">
@@ -12154,7 +12154,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C102">
@@ -12286,7 +12286,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C103">
@@ -12454,7 +12454,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C104">
@@ -12583,7 +12583,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C105">
@@ -12673,7 +12673,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C106">
@@ -12970,7 +12970,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C108">
@@ -13138,7 +13138,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C109">
@@ -13357,7 +13357,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C111">
@@ -13654,7 +13654,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C113">
@@ -14134,7 +14134,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C117">
@@ -14266,7 +14266,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C118">
@@ -14446,7 +14446,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C120">
@@ -14743,7 +14743,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C122">
@@ -14797,7 +14797,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C123">
@@ -15013,7 +15013,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C125">
@@ -15181,7 +15181,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C126">
@@ -15439,7 +15439,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C128">
@@ -15490,7 +15490,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C129">
@@ -15658,7 +15658,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C130">
@@ -15826,7 +15826,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C131">
@@ -16252,7 +16252,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C134">
@@ -16381,7 +16381,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C135">
@@ -16549,7 +16549,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C136">
@@ -16717,7 +16717,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C137">
@@ -16831,7 +16831,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C138">
@@ -16882,7 +16882,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C139">
@@ -17011,7 +17011,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C140">
@@ -17140,7 +17140,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C141">
@@ -17320,7 +17320,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C143">
@@ -17371,7 +17371,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C144">
@@ -17668,7 +17668,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C146">
@@ -17719,7 +17719,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C147">
@@ -17887,7 +17887,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C148">
@@ -18067,7 +18067,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C150">
@@ -18118,7 +18118,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C151">
@@ -18475,7 +18475,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C154">
@@ -18733,7 +18733,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C156">
@@ -19159,7 +19159,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C159">
@@ -19378,7 +19378,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C161">
@@ -19675,7 +19675,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C163">
@@ -19765,7 +19765,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C164">
@@ -19819,7 +19819,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C165">
@@ -19987,7 +19987,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C166">
@@ -20116,7 +20116,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C167">
@@ -20284,7 +20284,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C168">
@@ -20413,7 +20413,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C169">
@@ -21067,7 +21067,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C174">
@@ -21235,7 +21235,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C175">
@@ -21325,7 +21325,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C176">
@@ -22021,7 +22021,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C182">
@@ -22150,7 +22150,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C183">
@@ -22201,7 +22201,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C184">
@@ -22339,7 +22339,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C185">
@@ -22597,7 +22597,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C187">
@@ -22765,7 +22765,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C188">
@@ -22855,7 +22855,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C189">
@@ -22915,7 +22915,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C190">
@@ -23083,7 +23083,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C191">
@@ -23209,7 +23209,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C192">
@@ -23377,7 +23377,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C193">
@@ -23506,7 +23506,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C194">
@@ -23635,7 +23635,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C195">
@@ -23893,7 +23893,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C197">
@@ -24022,7 +24022,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C198">
@@ -24409,7 +24409,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C201">
@@ -24577,7 +24577,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C202">
@@ -24628,7 +24628,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C203">
@@ -24718,7 +24718,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C204">
@@ -24886,7 +24886,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>selfhelp</t>
+          <t>unguided</t>
         </is>
       </c>
       <c r="C205">
@@ -25054,7 +25054,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>guided</t>
         </is>
       </c>
       <c r="C206">

</xml_diff>